<commit_message>
stopped on working weeks
</commit_message>
<xml_diff>
--- a/Prepare Excel/dfTemplate.xlsx
+++ b/Prepare Excel/dfTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkowalc\Desktop\Python\Work\RemoteHWReservationSheet\Prepare Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027487ED-F6E4-4E05-BC76-D2AABFBEE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D658DF04-DF96-4800-8835-2B99BB4932E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32730" yWindow="2505" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Only migrating txt file left
</commit_message>
<xml_diff>
--- a/Prepare Excel/dfTemplate.xlsx
+++ b/Prepare Excel/dfTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkowalc\Desktop\Python\Work\RemoteHWReservationSheet\Prepare Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D658DF04-DF96-4800-8835-2B99BB4932E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA863EF-FB1C-4E67-9B01-F981E3F04401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32730" yWindow="2505" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36930" yWindow="1425" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Monday</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>After 18:00</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +522,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>